<commit_message>
Updating Model to Predict Both Priority Index and Is Emergengy Flag.
</commit_message>
<xml_diff>
--- a/data/Priority.xlsx
+++ b/data/Priority.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verge\Downloads\Cursos\Fusemachines - AI Fellowship Latam\FinalProject\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ana Verges\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C3E37E-B445-44AD-9967-DD4DB6F15771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3241562A-91D4-4510-A38F-4DC52B919851}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -923,7 +923,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1105,105 +1105,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCFE2F3"/>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCFE2F3"/>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCFE2F3"/>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1426,6 +1327,105 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1440,18 +1440,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DE07F371-B1DB-4ECA-95A9-FA0504A4E68E}" name="Table1" displayName="Table1" ref="A1:E144" totalsRowShown="0" headerRowDxfId="0" dataDxfId="19" headerRowBorderDxfId="1" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DE07F371-B1DB-4ECA-95A9-FA0504A4E68E}" name="Table1" displayName="Table1" ref="A1:E144" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:E144" xr:uid="{DE07F371-B1DB-4ECA-95A9-FA0504A4E68E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E144">
+  <sortState ref="A2:E144">
     <sortCondition ref="A2:A144"/>
     <sortCondition ref="C2:C144"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{95DF0D64-D48F-4771-B580-0B1E7A6E5258}" name="Type" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{932DD1E0-A3A1-41CA-8372-93DEB28E1831}" name="Name" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{5C8DCFE0-E446-428D-8AA5-514E4644A637}" name="Label" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{CDC79409-6A23-4507-939F-1F2973CE9D39}" name="Gender" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{D57E060E-C83C-44A5-8BA6-8D7ACB5A6FAF}" name="Priority" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{95DF0D64-D48F-4771-B580-0B1E7A6E5258}" name="Type" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{932DD1E0-A3A1-41CA-8372-93DEB28E1831}" name="Name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{5C8DCFE0-E446-428D-8AA5-514E4644A637}" name="Label" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{CDC79409-6A23-4507-939F-1F2973CE9D39}" name="Gender" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D57E060E-C83C-44A5-8BA6-8D7ACB5A6FAF}" name="Priority" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1660,20 +1660,20 @@
   </sheetPr>
   <dimension ref="A1:M751"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>145</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>152</v>
       </c>
@@ -1704,10 +1704,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>152</v>
       </c>
@@ -1721,10 +1721,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>152</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>152</v>
       </c>
@@ -1755,10 +1755,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>152</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>152</v>
       </c>
@@ -1789,10 +1789,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>152</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>152</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>152</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>154</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>154</v>
       </c>
@@ -1874,10 +1874,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>154</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>154</v>
       </c>
@@ -1908,10 +1908,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>154</v>
       </c>
@@ -1925,11 +1925,11 @@
         <v>1</v>
       </c>
       <c r="E15" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>154</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>154</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>154</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>154</v>
       </c>
@@ -1994,10 +1994,10 @@
         <v>1</v>
       </c>
       <c r="E19" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>154</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>154</v>
       </c>
@@ -2028,10 +2028,10 @@
         <v>1</v>
       </c>
       <c r="E21" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>154</v>
       </c>
@@ -2045,10 +2045,10 @@
         <v>1</v>
       </c>
       <c r="E22" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>154</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>154</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>155</v>
       </c>
@@ -2096,10 +2096,10 @@
         <v>1</v>
       </c>
       <c r="E25" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>155</v>
       </c>
@@ -2113,10 +2113,10 @@
         <v>1</v>
       </c>
       <c r="E26" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>155</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>155</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>155</v>
       </c>
@@ -2164,10 +2164,10 @@
         <v>1</v>
       </c>
       <c r="E29" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>155</v>
       </c>
@@ -2181,10 +2181,10 @@
         <v>1</v>
       </c>
       <c r="E30" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>155</v>
       </c>
@@ -2198,10 +2198,10 @@
         <v>1</v>
       </c>
       <c r="E31" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>155</v>
       </c>
@@ -2215,10 +2215,10 @@
         <v>1</v>
       </c>
       <c r="E32" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>155</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="6" t="s">
         <v>155</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>155</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="6" t="s">
         <v>155</v>
       </c>
@@ -2283,10 +2283,10 @@
         <v>1</v>
       </c>
       <c r="E36" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>155</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" s="6" t="s">
         <v>150</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="6" t="s">
         <v>150</v>
       </c>
@@ -2334,10 +2334,10 @@
         <v>1</v>
       </c>
       <c r="E39" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="6" t="s">
         <v>150</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="6" t="s">
         <v>150</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>150</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="6" t="s">
         <v>150</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1">
       <c r="A44" s="6" t="s">
         <v>150</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
       <c r="A45" s="6" t="s">
         <v>150</v>
       </c>
@@ -2436,10 +2436,10 @@
         <v>1</v>
       </c>
       <c r="E45" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1">
       <c r="A46" s="6" t="s">
         <v>150</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1">
       <c r="A47" s="6" t="s">
         <v>150</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1">
       <c r="A48" s="6" t="s">
         <v>150</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1">
       <c r="A49" s="6" t="s">
         <v>150</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1">
       <c r="A50" s="6" t="s">
         <v>150</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="A51" s="6" t="s">
         <v>150</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="A52" s="6" t="s">
         <v>150</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1">
       <c r="A53" s="6" t="s">
         <v>150</v>
       </c>
@@ -2572,10 +2572,10 @@
         <v>1</v>
       </c>
       <c r="E53" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1">
       <c r="A54" s="6" t="s">
         <v>150</v>
       </c>
@@ -2589,10 +2589,10 @@
         <v>1</v>
       </c>
       <c r="E54" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1">
       <c r="A55" s="6" t="s">
         <v>150</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="15.75" customHeight="1">
       <c r="A56" s="6" t="s">
         <v>150</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="15.75" customHeight="1">
       <c r="A57" s="6" t="s">
         <v>150</v>
       </c>
@@ -2640,10 +2640,10 @@
         <v>1</v>
       </c>
       <c r="E57" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1">
       <c r="A58" s="6" t="s">
         <v>150</v>
       </c>
@@ -2657,10 +2657,10 @@
         <v>1</v>
       </c>
       <c r="E58" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1">
       <c r="A59" s="6" t="s">
         <v>150</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="15.75" customHeight="1">
       <c r="A60" s="6" t="s">
         <v>150</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1">
       <c r="A61" s="6" t="s">
         <v>150</v>
       </c>
@@ -2708,10 +2708,10 @@
         <v>1</v>
       </c>
       <c r="E61" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" customHeight="1">
       <c r="A62" s="6" t="s">
         <v>150</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1">
       <c r="A63" s="6" t="s">
         <v>150</v>
       </c>
@@ -2742,10 +2742,10 @@
         <v>1</v>
       </c>
       <c r="E63" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" customHeight="1">
       <c r="A64" s="6" t="s">
         <v>150</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1">
       <c r="A65" s="6" t="s">
         <v>150</v>
       </c>
@@ -2776,10 +2776,10 @@
         <v>1</v>
       </c>
       <c r="E65" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1">
       <c r="A66" s="6" t="s">
         <v>150</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1">
       <c r="A67" s="6" t="s">
         <v>150</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1">
       <c r="A68" s="6" t="s">
         <v>150</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1">
       <c r="A69" s="6" t="s">
         <v>150</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1">
       <c r="A70" s="6" t="s">
         <v>150</v>
       </c>
@@ -2861,10 +2861,10 @@
         <v>1</v>
       </c>
       <c r="E70" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" customHeight="1">
       <c r="A71" s="6" t="s">
         <v>150</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1">
       <c r="A72" s="6" t="s">
         <v>150</v>
       </c>
@@ -2895,10 +2895,10 @@
         <v>1</v>
       </c>
       <c r="E72" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" customHeight="1">
       <c r="A73" s="6" t="s">
         <v>150</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1">
       <c r="A74" s="6" t="s">
         <v>150</v>
       </c>
@@ -2929,10 +2929,10 @@
         <v>1</v>
       </c>
       <c r="E74" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" customHeight="1">
       <c r="A75" s="6" t="s">
         <v>150</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1">
       <c r="A76" s="6" t="s">
         <v>150</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1">
       <c r="A77" s="6" t="s">
         <v>150</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1">
       <c r="A78" s="6" t="s">
         <v>150</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1">
       <c r="A79" s="6" t="s">
         <v>150</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1">
       <c r="A80" s="6" t="s">
         <v>150</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1">
       <c r="A81" s="6" t="s">
         <v>150</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1">
       <c r="A82" s="6" t="s">
         <v>150</v>
       </c>
@@ -3065,10 +3065,10 @@
         <v>1</v>
       </c>
       <c r="E82" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" customHeight="1">
       <c r="A83" s="6" t="s">
         <v>150</v>
       </c>
@@ -3082,10 +3082,10 @@
         <v>1</v>
       </c>
       <c r="E83" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" customHeight="1">
       <c r="A84" s="6" t="s">
         <v>150</v>
       </c>
@@ -3099,10 +3099,10 @@
         <v>1</v>
       </c>
       <c r="E84" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" customHeight="1">
       <c r="A85" s="6" t="s">
         <v>150</v>
       </c>
@@ -3116,10 +3116,10 @@
         <v>1</v>
       </c>
       <c r="E85" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" customHeight="1">
       <c r="A86" s="6" t="s">
         <v>150</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1">
       <c r="A87" s="6" t="s">
         <v>150</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1">
       <c r="A88" s="6" t="s">
         <v>150</v>
       </c>
@@ -3167,10 +3167,10 @@
         <v>1</v>
       </c>
       <c r="E88" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15.75" customHeight="1">
       <c r="A89" s="6" t="s">
         <v>150</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1">
       <c r="A90" s="6" t="s">
         <v>150</v>
       </c>
@@ -3201,10 +3201,10 @@
         <v>1</v>
       </c>
       <c r="E90" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" customHeight="1">
       <c r="A91" s="6" t="s">
         <v>150</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1">
       <c r="A92" s="6" t="s">
         <v>150</v>
       </c>
@@ -3235,10 +3235,10 @@
         <v>1</v>
       </c>
       <c r="E92" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" customHeight="1">
       <c r="A93" s="6" t="s">
         <v>150</v>
       </c>
@@ -3252,10 +3252,10 @@
         <v>1</v>
       </c>
       <c r="E93" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" customHeight="1">
       <c r="A94" s="6" t="s">
         <v>150</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1">
       <c r="A95" s="6" t="s">
         <v>150</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1">
       <c r="A96" s="6" t="s">
         <v>150</v>
       </c>
@@ -3303,10 +3303,10 @@
         <v>1</v>
       </c>
       <c r="E96" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" customHeight="1">
       <c r="A97" s="6" t="s">
         <v>150</v>
       </c>
@@ -3320,10 +3320,10 @@
         <v>1</v>
       </c>
       <c r="E97" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" customHeight="1">
       <c r="A98" s="6" t="s">
         <v>150</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1">
       <c r="A99" s="6" t="s">
         <v>150</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1">
       <c r="A100" s="6" t="s">
         <v>150</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1">
       <c r="A101" s="6" t="s">
         <v>150</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1">
       <c r="A102" s="6" t="s">
         <v>150</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" ht="13.2">
       <c r="A103" s="6" t="s">
         <v>150</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" ht="13.2">
       <c r="A104" s="6" t="s">
         <v>150</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" ht="13.2">
       <c r="A105" s="6" t="s">
         <v>150</v>
       </c>
@@ -3456,10 +3456,10 @@
         <v>1</v>
       </c>
       <c r="E105" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="13.2">
       <c r="A106" s="6" t="s">
         <v>150</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" ht="13.2">
       <c r="A107" s="6" t="s">
         <v>150</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" ht="13.2">
       <c r="A108" s="6" t="s">
         <v>150</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" ht="13.2">
       <c r="A109" s="6" t="s">
         <v>150</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" ht="13.2">
       <c r="A110" s="6" t="s">
         <v>150</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" ht="13.2">
       <c r="A111" s="6" t="s">
         <v>150</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" ht="13.2">
       <c r="A112" s="6" t="s">
         <v>150</v>
       </c>
@@ -3575,10 +3575,10 @@
         <v>1</v>
       </c>
       <c r="E112" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="13.2">
       <c r="A113" s="6" t="s">
         <v>150</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" ht="13.2">
       <c r="A114" s="6" t="s">
         <v>150</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" ht="13.2">
       <c r="A115" s="6" t="s">
         <v>150</v>
       </c>
@@ -3626,10 +3626,10 @@
         <v>1</v>
       </c>
       <c r="E115" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="13.2">
       <c r="A116" s="6" t="s">
         <v>150</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" ht="13.2">
       <c r="A117" s="6" t="s">
         <v>150</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" ht="13.2">
       <c r="A118" s="6" t="s">
         <v>150</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" ht="13.2">
       <c r="A119" s="6" t="s">
         <v>150</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" ht="13.2">
       <c r="A120" s="6" t="s">
         <v>150</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" ht="13.2">
       <c r="A121" s="6" t="s">
         <v>150</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" ht="13.2">
       <c r="A122" s="6" t="s">
         <v>150</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" ht="13.2">
       <c r="A123" s="6" t="s">
         <v>150</v>
       </c>
@@ -3762,10 +3762,10 @@
         <v>1</v>
       </c>
       <c r="E123" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="13.2">
       <c r="A124" s="6" t="s">
         <v>150</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" ht="13.2">
       <c r="A125" s="6" t="s">
         <v>150</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" ht="13.2">
       <c r="A126" s="6" t="s">
         <v>150</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" ht="13.2">
       <c r="A127" s="6" t="s">
         <v>153</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" ht="13.2">
       <c r="A128" s="6" t="s">
         <v>153</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="13.2">
       <c r="A129" s="6" t="s">
         <v>153</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" ht="13.2">
       <c r="A130" s="6" t="s">
         <v>153</v>
       </c>
@@ -3881,10 +3881,10 @@
         <v>115</v>
       </c>
       <c r="E130" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="13.2">
       <c r="A131" s="6" t="s">
         <v>153</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" ht="13.2">
       <c r="A132" s="6" t="s">
         <v>153</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" ht="13.2">
       <c r="A133" s="6" t="s">
         <v>151</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" ht="13.2">
       <c r="A134" s="6" t="s">
         <v>151</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" ht="13.2">
       <c r="A135" s="6" t="s">
         <v>151</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" ht="13.2">
       <c r="A136" s="6" t="s">
         <v>151</v>
       </c>
@@ -3983,10 +3983,10 @@
         <v>1</v>
       </c>
       <c r="E136" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="13.2">
       <c r="A137" s="6" t="s">
         <v>151</v>
       </c>
@@ -4000,10 +4000,10 @@
         <v>1</v>
       </c>
       <c r="E137" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="13.2">
       <c r="A138" s="6" t="s">
         <v>151</v>
       </c>
@@ -4017,10 +4017,10 @@
         <v>1</v>
       </c>
       <c r="E138" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="13.2">
       <c r="A139" s="6" t="s">
         <v>151</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" ht="13.2">
       <c r="A140" s="6" t="s">
         <v>151</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" ht="13.2">
       <c r="A141" s="6" t="s">
         <v>151</v>
       </c>
@@ -4068,11 +4068,11 @@
         <v>1</v>
       </c>
       <c r="E141" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I141" s="4"/>
     </row>
-    <row r="142" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" ht="13.2">
       <c r="A142" s="6" t="s">
         <v>151</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" ht="13.2">
       <c r="A143" s="6" t="s">
         <v>151</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" ht="13.2">
       <c r="A144" s="11" t="s">
         <v>151</v>
       </c>
@@ -4123,1829 +4123,1829 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" ht="13.2">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
       <c r="E145" s="2"/>
     </row>
-    <row r="146" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" ht="13.2">
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" ht="13.2">
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" ht="13.2">
       <c r="D148" s="2"/>
     </row>
-    <row r="149" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" ht="13.2">
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" ht="13.2">
       <c r="D150" s="2"/>
     </row>
-    <row r="151" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" ht="13.2">
       <c r="D151" s="2"/>
     </row>
-    <row r="152" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" ht="13.2">
       <c r="D152" s="2"/>
     </row>
-    <row r="153" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" ht="13.2">
       <c r="D153" s="2"/>
     </row>
-    <row r="154" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" ht="13.2">
       <c r="D154" s="2"/>
     </row>
-    <row r="155" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" ht="13.2">
       <c r="D155" s="2"/>
     </row>
-    <row r="156" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" ht="13.2">
       <c r="D156" s="2"/>
     </row>
-    <row r="157" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" ht="13.2">
       <c r="D157" s="2"/>
     </row>
-    <row r="158" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" ht="13.2">
       <c r="D158" s="2"/>
     </row>
-    <row r="159" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" ht="13.2">
       <c r="D159" s="2"/>
     </row>
-    <row r="160" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" ht="13.2">
       <c r="D160" s="2"/>
     </row>
-    <row r="161" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="4:4" ht="13.2">
       <c r="D161" s="2"/>
     </row>
-    <row r="162" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="4:4" ht="13.2">
       <c r="D162" s="2"/>
     </row>
-    <row r="163" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="4:4" ht="13.2">
       <c r="D163" s="2"/>
     </row>
-    <row r="164" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="4:4" ht="13.2">
       <c r="D164" s="2"/>
     </row>
-    <row r="165" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="4:4" ht="13.2">
       <c r="D165" s="2"/>
     </row>
-    <row r="166" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="4:4" ht="13.2">
       <c r="D166" s="2"/>
     </row>
-    <row r="167" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="4:4" ht="13.2">
       <c r="D167" s="2"/>
     </row>
-    <row r="168" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="4:4" ht="13.2">
       <c r="D168" s="2"/>
     </row>
-    <row r="169" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="4:4" ht="13.2">
       <c r="D169" s="2"/>
     </row>
-    <row r="170" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="4:4" ht="13.2">
       <c r="D170" s="2"/>
     </row>
-    <row r="171" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="4:4" ht="13.2">
       <c r="D171" s="2"/>
     </row>
-    <row r="172" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="4:4" ht="13.2">
       <c r="D172" s="2"/>
     </row>
-    <row r="173" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="4:4" ht="13.2">
       <c r="D173" s="2"/>
     </row>
-    <row r="174" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="4:4" ht="13.2">
       <c r="D174" s="2"/>
     </row>
-    <row r="175" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="4:4" ht="13.2">
       <c r="D175" s="2"/>
     </row>
-    <row r="176" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="4:4" ht="13.2">
       <c r="D176" s="2"/>
     </row>
-    <row r="177" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="4:4" ht="13.2">
       <c r="D177" s="2"/>
     </row>
-    <row r="178" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="4:4" ht="13.2">
       <c r="D178" s="2"/>
     </row>
-    <row r="179" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="4:4" ht="13.2">
       <c r="D179" s="2"/>
     </row>
-    <row r="180" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="4:4" ht="13.2">
       <c r="D180" s="2"/>
     </row>
-    <row r="181" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="4:4" ht="13.2">
       <c r="D181" s="2"/>
     </row>
-    <row r="182" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="4:4" ht="13.2">
       <c r="D182" s="2"/>
     </row>
-    <row r="183" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="4:4" ht="13.2">
       <c r="D183" s="2"/>
     </row>
-    <row r="184" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="4:4" ht="13.2">
       <c r="D184" s="2"/>
     </row>
-    <row r="185" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="4:4" ht="13.2">
       <c r="D185" s="2"/>
     </row>
-    <row r="186" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="4:4" ht="13.2">
       <c r="D186" s="2"/>
     </row>
-    <row r="187" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="4:4" ht="13.2">
       <c r="D187" s="2"/>
     </row>
-    <row r="188" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="4:4" ht="13.2">
       <c r="D188" s="2"/>
     </row>
-    <row r="189" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="4:4" ht="13.2">
       <c r="D189" s="2"/>
     </row>
-    <row r="190" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="4:4" ht="13.2">
       <c r="D190" s="2"/>
     </row>
-    <row r="191" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="4:4" ht="13.2">
       <c r="D191" s="2"/>
     </row>
-    <row r="192" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="4:4" ht="13.2">
       <c r="D192" s="2"/>
     </row>
-    <row r="193" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="4:4" ht="13.2">
       <c r="D193" s="2"/>
     </row>
-    <row r="194" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="4:4" ht="13.2">
       <c r="D194" s="2"/>
     </row>
-    <row r="195" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="4:4" ht="13.2">
       <c r="D195" s="2"/>
     </row>
-    <row r="196" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="4:4" ht="13.2">
       <c r="D196" s="2"/>
     </row>
-    <row r="197" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="4:4" ht="13.2">
       <c r="D197" s="2"/>
     </row>
-    <row r="198" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="4:4" ht="13.2">
       <c r="D198" s="2"/>
     </row>
-    <row r="199" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="4:4" ht="13.2">
       <c r="D199" s="2"/>
     </row>
-    <row r="200" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="4:4" ht="13.2">
       <c r="D200" s="2"/>
     </row>
-    <row r="201" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="4:4" ht="13.2">
       <c r="D201" s="2"/>
     </row>
-    <row r="202" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="4:4" ht="13.2">
       <c r="D202" s="2"/>
     </row>
-    <row r="203" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="4:4" ht="13.2">
       <c r="D203" s="2"/>
     </row>
-    <row r="204" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="4:4" ht="13.2">
       <c r="D204" s="2"/>
     </row>
-    <row r="205" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="4:4" ht="13.2">
       <c r="D205" s="2"/>
     </row>
-    <row r="206" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="4:4" ht="13.2">
       <c r="D206" s="2"/>
     </row>
-    <row r="207" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="4:4" ht="13.2">
       <c r="D207" s="2"/>
     </row>
-    <row r="208" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="4:4" ht="13.2">
       <c r="D208" s="2"/>
     </row>
-    <row r="209" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="4:4" ht="13.2">
       <c r="D209" s="2"/>
     </row>
-    <row r="210" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="4:4" ht="13.2">
       <c r="D210" s="2"/>
     </row>
-    <row r="211" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="4:4" ht="13.2">
       <c r="D211" s="2"/>
     </row>
-    <row r="212" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="4:4" ht="13.2">
       <c r="D212" s="2"/>
     </row>
-    <row r="213" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="4:4" ht="13.2">
       <c r="D213" s="2"/>
     </row>
-    <row r="214" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="214" spans="4:4" ht="13.2">
       <c r="D214" s="2"/>
     </row>
-    <row r="215" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="4:4" ht="13.2">
       <c r="D215" s="2"/>
     </row>
-    <row r="216" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="4:4" ht="13.2">
       <c r="D216" s="2"/>
     </row>
-    <row r="217" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="4:4" ht="13.2">
       <c r="D217" s="2"/>
     </row>
-    <row r="218" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="218" spans="4:4" ht="13.2">
       <c r="D218" s="2"/>
     </row>
-    <row r="219" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="219" spans="4:4" ht="13.2">
       <c r="D219" s="2"/>
     </row>
-    <row r="220" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="4:4" ht="13.2">
       <c r="D220" s="2"/>
     </row>
-    <row r="221" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="4:4" ht="13.2">
       <c r="D221" s="2"/>
     </row>
-    <row r="222" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="222" spans="4:4" ht="13.2">
       <c r="D222" s="2"/>
     </row>
-    <row r="223" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="4:4" ht="13.2">
       <c r="D223" s="2"/>
     </row>
-    <row r="224" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="224" spans="4:4" ht="13.2">
       <c r="D224" s="2"/>
     </row>
-    <row r="225" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="4:4" ht="13.2">
       <c r="D225" s="2"/>
     </row>
-    <row r="226" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="4:4" ht="13.2">
       <c r="D226" s="2"/>
     </row>
-    <row r="227" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="4:4" ht="13.2">
       <c r="D227" s="2"/>
     </row>
-    <row r="228" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="228" spans="4:4" ht="13.2">
       <c r="D228" s="2"/>
     </row>
-    <row r="229" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="229" spans="4:4" ht="13.2">
       <c r="D229" s="2"/>
     </row>
-    <row r="230" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="4:4" ht="13.2">
       <c r="D230" s="2"/>
     </row>
-    <row r="231" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="4:4" ht="13.2">
       <c r="D231" s="2"/>
     </row>
-    <row r="232" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="4:4" ht="13.2">
       <c r="D232" s="2"/>
     </row>
-    <row r="233" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="4:4" ht="13.2">
       <c r="D233" s="2"/>
     </row>
-    <row r="234" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="4:4" ht="13.2">
       <c r="D234" s="2"/>
     </row>
-    <row r="235" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="4:4" ht="13.2">
       <c r="D235" s="2"/>
     </row>
-    <row r="236" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="236" spans="4:4" ht="13.2">
       <c r="D236" s="2"/>
     </row>
-    <row r="237" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="4:4" ht="13.2">
       <c r="D237" s="2"/>
     </row>
-    <row r="238" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="4:4" ht="13.2">
       <c r="D238" s="2"/>
     </row>
-    <row r="239" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="4:4" ht="13.2">
       <c r="D239" s="2"/>
     </row>
-    <row r="240" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="240" spans="4:4" ht="13.2">
       <c r="D240" s="2"/>
     </row>
-    <row r="241" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="4:4" ht="13.2">
       <c r="D241" s="2"/>
     </row>
-    <row r="242" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="4:4" ht="13.2">
       <c r="D242" s="2"/>
     </row>
-    <row r="243" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="4:4" ht="13.2">
       <c r="D243" s="2"/>
     </row>
-    <row r="244" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="244" spans="4:4" ht="13.2">
       <c r="D244" s="2"/>
     </row>
-    <row r="245" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="245" spans="4:4" ht="13.2">
       <c r="D245" s="2"/>
     </row>
-    <row r="246" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="4:4" ht="13.2">
       <c r="D246" s="2"/>
     </row>
-    <row r="247" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="247" spans="4:4" ht="13.2">
       <c r="D247" s="2"/>
     </row>
-    <row r="248" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="248" spans="4:4" ht="13.2">
       <c r="D248" s="2"/>
     </row>
-    <row r="249" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="249" spans="4:4" ht="13.2">
       <c r="D249" s="2"/>
     </row>
-    <row r="250" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="250" spans="4:4" ht="13.2">
       <c r="D250" s="2"/>
     </row>
-    <row r="251" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="251" spans="4:4" ht="13.2">
       <c r="D251" s="2"/>
     </row>
-    <row r="252" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="252" spans="4:4" ht="13.2">
       <c r="D252" s="2"/>
     </row>
-    <row r="253" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="253" spans="4:4" ht="13.2">
       <c r="D253" s="2"/>
     </row>
-    <row r="254" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="254" spans="4:4" ht="13.2">
       <c r="D254" s="2"/>
     </row>
-    <row r="255" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="255" spans="4:4" ht="13.2">
       <c r="D255" s="2"/>
     </row>
-    <row r="256" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="256" spans="4:4" ht="13.2">
       <c r="D256" s="2"/>
     </row>
-    <row r="257" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="257" spans="4:4" ht="13.2">
       <c r="D257" s="2"/>
     </row>
-    <row r="258" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="258" spans="4:4" ht="13.2">
       <c r="D258" s="2"/>
     </row>
-    <row r="259" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="259" spans="4:4" ht="13.2">
       <c r="D259" s="2"/>
     </row>
-    <row r="260" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="260" spans="4:4" ht="13.2">
       <c r="D260" s="2"/>
     </row>
-    <row r="261" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="261" spans="4:4" ht="13.2">
       <c r="D261" s="2"/>
     </row>
-    <row r="262" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="262" spans="4:4" ht="13.2">
       <c r="D262" s="2"/>
     </row>
-    <row r="263" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="4:4" ht="13.2">
       <c r="D263" s="2"/>
     </row>
-    <row r="264" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="264" spans="4:4" ht="13.2">
       <c r="D264" s="2"/>
     </row>
-    <row r="265" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="265" spans="4:4" ht="13.2">
       <c r="D265" s="2"/>
     </row>
-    <row r="266" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="266" spans="4:4" ht="13.2">
       <c r="D266" s="2"/>
     </row>
-    <row r="267" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="267" spans="4:4" ht="13.2">
       <c r="D267" s="2"/>
     </row>
-    <row r="268" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="268" spans="4:4" ht="13.2">
       <c r="D268" s="2"/>
     </row>
-    <row r="269" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="269" spans="4:4" ht="13.2">
       <c r="D269" s="2"/>
     </row>
-    <row r="270" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="270" spans="4:4" ht="13.2">
       <c r="D270" s="2"/>
     </row>
-    <row r="271" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="271" spans="4:4" ht="13.2">
       <c r="D271" s="2"/>
     </row>
-    <row r="272" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="272" spans="4:4" ht="13.2">
       <c r="D272" s="2"/>
     </row>
-    <row r="273" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="273" spans="4:4" ht="13.2">
       <c r="D273" s="2"/>
     </row>
-    <row r="274" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="274" spans="4:4" ht="13.2">
       <c r="D274" s="2"/>
     </row>
-    <row r="275" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="275" spans="4:4" ht="13.2">
       <c r="D275" s="2"/>
     </row>
-    <row r="276" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="276" spans="4:4" ht="13.2">
       <c r="D276" s="2"/>
     </row>
-    <row r="277" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="277" spans="4:4" ht="13.2">
       <c r="D277" s="2"/>
     </row>
-    <row r="278" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="278" spans="4:4" ht="13.2">
       <c r="D278" s="2"/>
     </row>
-    <row r="279" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="279" spans="4:4" ht="13.2">
       <c r="D279" s="2"/>
     </row>
-    <row r="280" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="280" spans="4:4" ht="13.2">
       <c r="D280" s="2"/>
     </row>
-    <row r="281" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="281" spans="4:4" ht="13.2">
       <c r="D281" s="2"/>
     </row>
-    <row r="282" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="282" spans="4:4" ht="13.2">
       <c r="D282" s="2"/>
     </row>
-    <row r="283" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="283" spans="4:4" ht="13.2">
       <c r="D283" s="2"/>
     </row>
-    <row r="284" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="284" spans="4:4" ht="13.2">
       <c r="D284" s="2"/>
     </row>
-    <row r="285" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="285" spans="4:4" ht="13.2">
       <c r="D285" s="2"/>
     </row>
-    <row r="286" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="286" spans="4:4" ht="13.2">
       <c r="D286" s="2"/>
     </row>
-    <row r="287" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="287" spans="4:4" ht="13.2">
       <c r="D287" s="2"/>
     </row>
-    <row r="288" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="288" spans="4:4" ht="13.2">
       <c r="D288" s="2"/>
     </row>
-    <row r="289" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="289" spans="4:4" ht="13.2">
       <c r="D289" s="2"/>
     </row>
-    <row r="290" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="290" spans="4:4" ht="13.2">
       <c r="D290" s="2"/>
     </row>
-    <row r="291" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="291" spans="4:4" ht="13.2">
       <c r="D291" s="2"/>
     </row>
-    <row r="292" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="292" spans="4:4" ht="13.2">
       <c r="D292" s="2"/>
     </row>
-    <row r="293" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="293" spans="4:4" ht="13.2">
       <c r="D293" s="2"/>
     </row>
-    <row r="294" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="294" spans="4:4" ht="13.2">
       <c r="D294" s="2"/>
     </row>
-    <row r="295" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="295" spans="4:4" ht="13.2">
       <c r="D295" s="2"/>
     </row>
-    <row r="296" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="296" spans="4:4" ht="13.2">
       <c r="D296" s="2"/>
     </row>
-    <row r="297" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="297" spans="4:4" ht="13.2">
       <c r="D297" s="2"/>
     </row>
-    <row r="298" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="298" spans="4:4" ht="13.2">
       <c r="D298" s="2"/>
     </row>
-    <row r="299" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="299" spans="4:4" ht="13.2">
       <c r="D299" s="2"/>
     </row>
-    <row r="300" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="300" spans="4:4" ht="13.2">
       <c r="D300" s="2"/>
     </row>
-    <row r="301" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="301" spans="4:4" ht="13.2">
       <c r="D301" s="2"/>
     </row>
-    <row r="302" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="302" spans="4:4" ht="13.2">
       <c r="D302" s="2"/>
     </row>
-    <row r="303" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="303" spans="4:4" ht="13.2">
       <c r="D303" s="2"/>
     </row>
-    <row r="304" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="304" spans="4:4" ht="13.2">
       <c r="D304" s="2"/>
     </row>
-    <row r="305" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="305" spans="4:4" ht="13.2">
       <c r="D305" s="2"/>
     </row>
-    <row r="306" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="306" spans="4:4" ht="13.2">
       <c r="D306" s="2"/>
     </row>
-    <row r="307" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="307" spans="4:4" ht="13.2">
       <c r="D307" s="2"/>
     </row>
-    <row r="308" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="308" spans="4:4" ht="13.2">
       <c r="D308" s="2"/>
     </row>
-    <row r="309" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="309" spans="4:4" ht="13.2">
       <c r="D309" s="2"/>
     </row>
-    <row r="310" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="310" spans="4:4" ht="13.2">
       <c r="D310" s="2"/>
     </row>
-    <row r="311" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="311" spans="4:4" ht="13.2">
       <c r="D311" s="2"/>
     </row>
-    <row r="312" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="312" spans="4:4" ht="13.2">
       <c r="D312" s="2"/>
     </row>
-    <row r="313" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="313" spans="4:4" ht="13.2">
       <c r="D313" s="2"/>
     </row>
-    <row r="314" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="314" spans="4:4" ht="13.2">
       <c r="D314" s="2"/>
     </row>
-    <row r="315" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="315" spans="4:4" ht="13.2">
       <c r="D315" s="2"/>
     </row>
-    <row r="316" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="316" spans="4:4" ht="13.2">
       <c r="D316" s="2"/>
     </row>
-    <row r="317" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="317" spans="4:4" ht="13.2">
       <c r="D317" s="2"/>
     </row>
-    <row r="318" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="318" spans="4:4" ht="13.2">
       <c r="D318" s="2"/>
     </row>
-    <row r="319" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="319" spans="4:4" ht="13.2">
       <c r="D319" s="2"/>
     </row>
-    <row r="320" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="320" spans="4:4" ht="13.2">
       <c r="D320" s="2"/>
     </row>
-    <row r="321" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="321" spans="4:4" ht="13.2">
       <c r="D321" s="2"/>
     </row>
-    <row r="322" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="322" spans="4:4" ht="13.2">
       <c r="D322" s="2"/>
     </row>
-    <row r="323" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="323" spans="4:4" ht="13.2">
       <c r="D323" s="2"/>
     </row>
-    <row r="324" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="324" spans="4:4" ht="13.2">
       <c r="D324" s="2"/>
     </row>
-    <row r="325" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="325" spans="4:4" ht="13.2">
       <c r="D325" s="2"/>
     </row>
-    <row r="326" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="326" spans="4:4" ht="13.2">
       <c r="D326" s="2"/>
     </row>
-    <row r="327" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="327" spans="4:4" ht="13.2">
       <c r="D327" s="2"/>
     </row>
-    <row r="328" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="328" spans="4:4" ht="13.2">
       <c r="D328" s="2"/>
     </row>
-    <row r="329" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="329" spans="4:4" ht="13.2">
       <c r="D329" s="2"/>
     </row>
-    <row r="330" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="330" spans="4:4" ht="13.2">
       <c r="D330" s="2"/>
     </row>
-    <row r="331" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="331" spans="4:4" ht="13.2">
       <c r="D331" s="2"/>
     </row>
-    <row r="332" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="332" spans="4:4" ht="13.2">
       <c r="D332" s="2"/>
     </row>
-    <row r="333" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="333" spans="4:4" ht="13.2">
       <c r="D333" s="2"/>
     </row>
-    <row r="334" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="334" spans="4:4" ht="13.2">
       <c r="D334" s="2"/>
     </row>
-    <row r="335" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="335" spans="4:4" ht="13.2">
       <c r="D335" s="2"/>
     </row>
-    <row r="336" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="336" spans="4:4" ht="13.2">
       <c r="D336" s="2"/>
     </row>
-    <row r="337" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="337" spans="4:4" ht="13.2">
       <c r="D337" s="2"/>
     </row>
-    <row r="338" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="338" spans="4:4" ht="13.2">
       <c r="D338" s="2"/>
     </row>
-    <row r="339" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="339" spans="4:4" ht="13.2">
       <c r="D339" s="2"/>
     </row>
-    <row r="340" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="340" spans="4:4" ht="13.2">
       <c r="D340" s="2"/>
     </row>
-    <row r="341" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="341" spans="4:4" ht="13.2">
       <c r="D341" s="2"/>
     </row>
-    <row r="342" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="342" spans="4:4" ht="13.2">
       <c r="D342" s="2"/>
     </row>
-    <row r="343" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="343" spans="4:4" ht="13.2">
       <c r="D343" s="2"/>
     </row>
-    <row r="344" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="344" spans="4:4" ht="13.2">
       <c r="D344" s="2"/>
     </row>
-    <row r="345" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="345" spans="4:4" ht="13.2">
       <c r="D345" s="2"/>
     </row>
-    <row r="346" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="346" spans="4:4" ht="13.2">
       <c r="D346" s="2"/>
     </row>
-    <row r="347" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="347" spans="4:4" ht="13.2">
       <c r="D347" s="2"/>
     </row>
-    <row r="348" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="348" spans="4:4" ht="13.2">
       <c r="D348" s="2"/>
     </row>
-    <row r="349" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="349" spans="4:4" ht="13.2">
       <c r="D349" s="2"/>
     </row>
-    <row r="350" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="350" spans="4:4" ht="13.2">
       <c r="D350" s="2"/>
     </row>
-    <row r="351" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="351" spans="4:4" ht="13.2">
       <c r="D351" s="2"/>
     </row>
-    <row r="352" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="352" spans="4:4" ht="13.2">
       <c r="D352" s="2"/>
     </row>
-    <row r="353" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="353" spans="4:4" ht="13.2">
       <c r="D353" s="2"/>
     </row>
-    <row r="354" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="354" spans="4:4" ht="13.2">
       <c r="D354" s="2"/>
     </row>
-    <row r="355" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="355" spans="4:4" ht="13.2">
       <c r="D355" s="2"/>
     </row>
-    <row r="356" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="356" spans="4:4" ht="13.2">
       <c r="D356" s="2"/>
     </row>
-    <row r="357" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="357" spans="4:4" ht="13.2">
       <c r="D357" s="2"/>
     </row>
-    <row r="358" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="358" spans="4:4" ht="13.2">
       <c r="D358" s="2"/>
     </row>
-    <row r="359" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="359" spans="4:4" ht="13.2">
       <c r="D359" s="2"/>
     </row>
-    <row r="360" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="360" spans="4:4" ht="13.2">
       <c r="D360" s="2"/>
     </row>
-    <row r="361" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="361" spans="4:4" ht="13.2">
       <c r="D361" s="2"/>
     </row>
-    <row r="362" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="362" spans="4:4" ht="13.2">
       <c r="D362" s="2"/>
     </row>
-    <row r="363" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="363" spans="4:4" ht="13.2">
       <c r="D363" s="2"/>
     </row>
-    <row r="364" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="364" spans="4:4" ht="13.2">
       <c r="D364" s="2"/>
     </row>
-    <row r="365" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="365" spans="4:4" ht="13.2">
       <c r="D365" s="2"/>
     </row>
-    <row r="366" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="366" spans="4:4" ht="13.2">
       <c r="D366" s="2"/>
     </row>
-    <row r="367" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="367" spans="4:4" ht="13.2">
       <c r="D367" s="2"/>
     </row>
-    <row r="368" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="368" spans="4:4" ht="13.2">
       <c r="D368" s="2"/>
     </row>
-    <row r="369" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="369" spans="4:4" ht="13.2">
       <c r="D369" s="2"/>
     </row>
-    <row r="370" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="370" spans="4:4" ht="13.2">
       <c r="D370" s="2"/>
     </row>
-    <row r="371" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="371" spans="4:4" ht="13.2">
       <c r="D371" s="2"/>
     </row>
-    <row r="372" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="372" spans="4:4" ht="13.2">
       <c r="D372" s="2"/>
     </row>
-    <row r="373" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="373" spans="4:4" ht="13.2">
       <c r="D373" s="2"/>
     </row>
-    <row r="374" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="374" spans="4:4" ht="13.2">
       <c r="D374" s="2"/>
     </row>
-    <row r="375" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="375" spans="4:4" ht="13.2">
       <c r="D375" s="2"/>
     </row>
-    <row r="376" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="376" spans="4:4" ht="13.2">
       <c r="D376" s="2"/>
     </row>
-    <row r="377" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="377" spans="4:4" ht="13.2">
       <c r="D377" s="2"/>
     </row>
-    <row r="378" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="378" spans="4:4" ht="13.2">
       <c r="D378" s="2"/>
     </row>
-    <row r="379" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="379" spans="4:4" ht="13.2">
       <c r="D379" s="2"/>
     </row>
-    <row r="380" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="380" spans="4:4" ht="13.2">
       <c r="D380" s="2"/>
     </row>
-    <row r="381" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="381" spans="4:4" ht="13.2">
       <c r="D381" s="2"/>
     </row>
-    <row r="382" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="382" spans="4:4" ht="13.2">
       <c r="D382" s="2"/>
     </row>
-    <row r="383" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="383" spans="4:4" ht="13.2">
       <c r="D383" s="2"/>
     </row>
-    <row r="384" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="384" spans="4:4" ht="13.2">
       <c r="D384" s="2"/>
     </row>
-    <row r="385" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="385" spans="4:4" ht="13.2">
       <c r="D385" s="2"/>
     </row>
-    <row r="386" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="386" spans="4:4" ht="13.2">
       <c r="D386" s="2"/>
     </row>
-    <row r="387" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="387" spans="4:4" ht="13.2">
       <c r="D387" s="2"/>
     </row>
-    <row r="388" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="388" spans="4:4" ht="13.2">
       <c r="D388" s="2"/>
     </row>
-    <row r="389" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="389" spans="4:4" ht="13.2">
       <c r="D389" s="2"/>
     </row>
-    <row r="390" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="390" spans="4:4" ht="13.2">
       <c r="D390" s="2"/>
     </row>
-    <row r="391" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="391" spans="4:4" ht="13.2">
       <c r="D391" s="2"/>
     </row>
-    <row r="392" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="392" spans="4:4" ht="13.2">
       <c r="D392" s="2"/>
     </row>
-    <row r="393" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="393" spans="4:4" ht="13.2">
       <c r="D393" s="2"/>
     </row>
-    <row r="394" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="394" spans="4:4" ht="13.2">
       <c r="D394" s="2"/>
     </row>
-    <row r="395" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="395" spans="4:4" ht="13.2">
       <c r="D395" s="2"/>
     </row>
-    <row r="396" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="396" spans="4:4" ht="13.2">
       <c r="D396" s="2"/>
     </row>
-    <row r="397" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="397" spans="4:4" ht="13.2">
       <c r="D397" s="2"/>
     </row>
-    <row r="398" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="398" spans="4:4" ht="13.2">
       <c r="D398" s="2"/>
     </row>
-    <row r="399" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="399" spans="4:4" ht="13.2">
       <c r="D399" s="2"/>
     </row>
-    <row r="400" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="400" spans="4:4" ht="13.2">
       <c r="D400" s="2"/>
     </row>
-    <row r="401" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="401" spans="4:4" ht="13.2">
       <c r="D401" s="2"/>
     </row>
-    <row r="402" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="402" spans="4:4" ht="13.2">
       <c r="D402" s="2"/>
     </row>
-    <row r="403" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="403" spans="4:4" ht="13.2">
       <c r="D403" s="2"/>
     </row>
-    <row r="404" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="404" spans="4:4" ht="13.2">
       <c r="D404" s="2"/>
     </row>
-    <row r="405" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="405" spans="4:4" ht="13.2">
       <c r="D405" s="2"/>
     </row>
-    <row r="406" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="406" spans="4:4" ht="13.2">
       <c r="D406" s="2"/>
     </row>
-    <row r="407" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="407" spans="4:4" ht="13.2">
       <c r="D407" s="2"/>
     </row>
-    <row r="408" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="408" spans="4:4" ht="13.2">
       <c r="D408" s="2"/>
     </row>
-    <row r="409" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="409" spans="4:4" ht="13.2">
       <c r="D409" s="2"/>
     </row>
-    <row r="410" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="410" spans="4:4" ht="13.2">
       <c r="D410" s="2"/>
     </row>
-    <row r="411" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="411" spans="4:4" ht="13.2">
       <c r="D411" s="2"/>
     </row>
-    <row r="412" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="412" spans="4:4" ht="13.2">
       <c r="D412" s="2"/>
     </row>
-    <row r="413" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="413" spans="4:4" ht="13.2">
       <c r="D413" s="2"/>
     </row>
-    <row r="414" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="414" spans="4:4" ht="13.2">
       <c r="D414" s="2"/>
     </row>
-    <row r="415" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="415" spans="4:4" ht="13.2">
       <c r="D415" s="2"/>
     </row>
-    <row r="416" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="416" spans="4:4" ht="13.2">
       <c r="D416" s="2"/>
     </row>
-    <row r="417" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="417" spans="4:4" ht="13.2">
       <c r="D417" s="2"/>
     </row>
-    <row r="418" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="418" spans="4:4" ht="13.2">
       <c r="D418" s="2"/>
     </row>
-    <row r="419" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="419" spans="4:4" ht="13.2">
       <c r="D419" s="2"/>
     </row>
-    <row r="420" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="420" spans="4:4" ht="13.2">
       <c r="D420" s="2"/>
     </row>
-    <row r="421" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="421" spans="4:4" ht="13.2">
       <c r="D421" s="2"/>
     </row>
-    <row r="422" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="422" spans="4:4" ht="13.2">
       <c r="D422" s="2"/>
     </row>
-    <row r="423" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="423" spans="4:4" ht="13.2">
       <c r="D423" s="2"/>
     </row>
-    <row r="424" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="424" spans="4:4" ht="13.2">
       <c r="D424" s="2"/>
     </row>
-    <row r="425" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="425" spans="4:4" ht="13.2">
       <c r="D425" s="2"/>
     </row>
-    <row r="426" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="426" spans="4:4" ht="13.2">
       <c r="D426" s="2"/>
     </row>
-    <row r="427" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="427" spans="4:4" ht="13.2">
       <c r="D427" s="2"/>
     </row>
-    <row r="428" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="428" spans="4:4" ht="13.2">
       <c r="D428" s="2"/>
     </row>
-    <row r="429" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="429" spans="4:4" ht="13.2">
       <c r="D429" s="2"/>
     </row>
-    <row r="430" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="430" spans="4:4" ht="13.2">
       <c r="D430" s="2"/>
     </row>
-    <row r="431" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="431" spans="4:4" ht="13.2">
       <c r="D431" s="2"/>
     </row>
-    <row r="432" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="432" spans="4:4" ht="13.2">
       <c r="D432" s="2"/>
     </row>
-    <row r="433" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="433" spans="4:4" ht="13.2">
       <c r="D433" s="2"/>
     </row>
-    <row r="434" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="434" spans="4:4" ht="13.2">
       <c r="D434" s="2"/>
     </row>
-    <row r="435" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="435" spans="4:4" ht="13.2">
       <c r="D435" s="2"/>
     </row>
-    <row r="436" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="436" spans="4:4" ht="13.2">
       <c r="D436" s="2"/>
     </row>
-    <row r="437" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="437" spans="4:4" ht="13.2">
       <c r="D437" s="2"/>
     </row>
-    <row r="438" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="438" spans="4:4" ht="13.2">
       <c r="D438" s="2"/>
     </row>
-    <row r="439" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="439" spans="4:4" ht="13.2">
       <c r="D439" s="2"/>
     </row>
-    <row r="440" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="440" spans="4:4" ht="13.2">
       <c r="D440" s="2"/>
     </row>
-    <row r="441" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="441" spans="4:4" ht="13.2">
       <c r="D441" s="2"/>
     </row>
-    <row r="442" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="442" spans="4:4" ht="13.2">
       <c r="D442" s="2"/>
     </row>
-    <row r="443" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="443" spans="4:4" ht="13.2">
       <c r="D443" s="2"/>
     </row>
-    <row r="444" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="444" spans="4:4" ht="13.2">
       <c r="D444" s="2"/>
     </row>
-    <row r="445" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="445" spans="4:4" ht="13.2">
       <c r="D445" s="2"/>
     </row>
-    <row r="446" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="446" spans="4:4" ht="13.2">
       <c r="D446" s="2"/>
     </row>
-    <row r="447" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="447" spans="4:4" ht="13.2">
       <c r="D447" s="2"/>
     </row>
-    <row r="448" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="448" spans="4:4" ht="13.2">
       <c r="D448" s="2"/>
     </row>
-    <row r="449" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="449" spans="4:4" ht="13.2">
       <c r="D449" s="2"/>
     </row>
-    <row r="450" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="450" spans="4:4" ht="13.2">
       <c r="D450" s="2"/>
     </row>
-    <row r="451" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="451" spans="4:4" ht="13.2">
       <c r="D451" s="2"/>
     </row>
-    <row r="452" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="452" spans="4:4" ht="13.2">
       <c r="D452" s="2"/>
     </row>
-    <row r="453" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="453" spans="4:4" ht="13.2">
       <c r="D453" s="2"/>
     </row>
-    <row r="454" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="454" spans="4:4" ht="13.2">
       <c r="D454" s="2"/>
     </row>
-    <row r="455" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="455" spans="4:4" ht="13.2">
       <c r="D455" s="2"/>
     </row>
-    <row r="456" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="456" spans="4:4" ht="13.2">
       <c r="D456" s="2"/>
     </row>
-    <row r="457" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="457" spans="4:4" ht="13.2">
       <c r="D457" s="2"/>
     </row>
-    <row r="458" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="458" spans="4:4" ht="13.2">
       <c r="D458" s="2"/>
     </row>
-    <row r="459" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="459" spans="4:4" ht="13.2">
       <c r="D459" s="2"/>
     </row>
-    <row r="460" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="460" spans="4:4" ht="13.2">
       <c r="D460" s="2"/>
     </row>
-    <row r="461" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="461" spans="4:4" ht="13.2">
       <c r="D461" s="2"/>
     </row>
-    <row r="462" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="462" spans="4:4" ht="13.2">
       <c r="D462" s="2"/>
     </row>
-    <row r="463" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="463" spans="4:4" ht="13.2">
       <c r="D463" s="2"/>
     </row>
-    <row r="464" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="464" spans="4:4" ht="13.2">
       <c r="D464" s="2"/>
     </row>
-    <row r="465" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="465" spans="4:4" ht="13.2">
       <c r="D465" s="2"/>
     </row>
-    <row r="466" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="466" spans="4:4" ht="13.2">
       <c r="D466" s="2"/>
     </row>
-    <row r="467" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="467" spans="4:4" ht="13.2">
       <c r="D467" s="2"/>
     </row>
-    <row r="468" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="468" spans="4:4" ht="13.2">
       <c r="D468" s="2"/>
     </row>
-    <row r="469" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="469" spans="4:4" ht="13.2">
       <c r="D469" s="2"/>
     </row>
-    <row r="470" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="470" spans="4:4" ht="13.2">
       <c r="D470" s="2"/>
     </row>
-    <row r="471" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="471" spans="4:4" ht="13.2">
       <c r="D471" s="2"/>
     </row>
-    <row r="472" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="472" spans="4:4" ht="13.2">
       <c r="D472" s="2"/>
     </row>
-    <row r="473" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="473" spans="4:4" ht="13.2">
       <c r="D473" s="2"/>
     </row>
-    <row r="474" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="474" spans="4:4" ht="13.2">
       <c r="D474" s="2"/>
     </row>
-    <row r="475" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="475" spans="4:4" ht="13.2">
       <c r="D475" s="2"/>
     </row>
-    <row r="476" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="476" spans="4:4" ht="13.2">
       <c r="D476" s="2"/>
     </row>
-    <row r="477" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="477" spans="4:4" ht="13.2">
       <c r="D477" s="2"/>
     </row>
-    <row r="478" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="478" spans="4:4" ht="13.2">
       <c r="D478" s="2"/>
     </row>
-    <row r="479" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="479" spans="4:4" ht="13.2">
       <c r="D479" s="2"/>
     </row>
-    <row r="480" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="480" spans="4:4" ht="13.2">
       <c r="D480" s="2"/>
     </row>
-    <row r="481" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="481" spans="4:4" ht="13.2">
       <c r="D481" s="2"/>
     </row>
-    <row r="482" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="482" spans="4:4" ht="13.2">
       <c r="D482" s="2"/>
     </row>
-    <row r="483" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="483" spans="4:4" ht="13.2">
       <c r="D483" s="2"/>
     </row>
-    <row r="484" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="484" spans="4:4" ht="13.2">
       <c r="D484" s="2"/>
     </row>
-    <row r="485" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="485" spans="4:4" ht="13.2">
       <c r="D485" s="2"/>
     </row>
-    <row r="486" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="486" spans="4:4" ht="13.2">
       <c r="D486" s="2"/>
     </row>
-    <row r="487" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="487" spans="4:4" ht="13.2">
       <c r="D487" s="2"/>
     </row>
-    <row r="488" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="488" spans="4:4" ht="13.2">
       <c r="D488" s="2"/>
     </row>
-    <row r="489" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="489" spans="4:4" ht="13.2">
       <c r="D489" s="2"/>
     </row>
-    <row r="490" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="490" spans="4:4" ht="13.2">
       <c r="D490" s="2"/>
     </row>
-    <row r="491" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="491" spans="4:4" ht="13.2">
       <c r="D491" s="2"/>
     </row>
-    <row r="492" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="492" spans="4:4" ht="13.2">
       <c r="D492" s="2"/>
     </row>
-    <row r="493" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="493" spans="4:4" ht="13.2">
       <c r="D493" s="2"/>
     </row>
-    <row r="494" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="494" spans="4:4" ht="13.2">
       <c r="D494" s="2"/>
     </row>
-    <row r="495" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="495" spans="4:4" ht="13.2">
       <c r="D495" s="2"/>
     </row>
-    <row r="496" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="496" spans="4:4" ht="13.2">
       <c r="D496" s="2"/>
     </row>
-    <row r="497" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="497" spans="4:4" ht="13.2">
       <c r="D497" s="2"/>
     </row>
-    <row r="498" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="498" spans="4:4" ht="13.2">
       <c r="D498" s="2"/>
     </row>
-    <row r="499" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="499" spans="4:4" ht="13.2">
       <c r="D499" s="2"/>
     </row>
-    <row r="500" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="500" spans="4:4" ht="13.2">
       <c r="D500" s="2"/>
     </row>
-    <row r="501" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="501" spans="4:4" ht="13.2">
       <c r="D501" s="2"/>
     </row>
-    <row r="502" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="502" spans="4:4" ht="13.2">
       <c r="D502" s="2"/>
     </row>
-    <row r="503" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="503" spans="4:4" ht="13.2">
       <c r="D503" s="2"/>
     </row>
-    <row r="504" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="504" spans="4:4" ht="13.2">
       <c r="D504" s="2"/>
     </row>
-    <row r="505" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="505" spans="4:4" ht="13.2">
       <c r="D505" s="2"/>
     </row>
-    <row r="506" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="506" spans="4:4" ht="13.2">
       <c r="D506" s="2"/>
     </row>
-    <row r="507" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="507" spans="4:4" ht="13.2">
       <c r="D507" s="2"/>
     </row>
-    <row r="508" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="508" spans="4:4" ht="13.2">
       <c r="D508" s="2"/>
     </row>
-    <row r="509" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="509" spans="4:4" ht="13.2">
       <c r="D509" s="2"/>
     </row>
-    <row r="510" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="510" spans="4:4" ht="13.2">
       <c r="D510" s="2"/>
     </row>
-    <row r="511" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="511" spans="4:4" ht="13.2">
       <c r="D511" s="2"/>
     </row>
-    <row r="512" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="512" spans="4:4" ht="13.2">
       <c r="D512" s="2"/>
     </row>
-    <row r="513" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="513" spans="4:4" ht="13.2">
       <c r="D513" s="2"/>
     </row>
-    <row r="514" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="514" spans="4:4" ht="13.2">
       <c r="D514" s="2"/>
     </row>
-    <row r="515" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="515" spans="4:4" ht="13.2">
       <c r="D515" s="2"/>
     </row>
-    <row r="516" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="516" spans="4:4" ht="13.2">
       <c r="D516" s="2"/>
     </row>
-    <row r="517" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="517" spans="4:4" ht="13.2">
       <c r="D517" s="2"/>
     </row>
-    <row r="518" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="518" spans="4:4" ht="13.2">
       <c r="D518" s="2"/>
     </row>
-    <row r="519" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="519" spans="4:4" ht="13.2">
       <c r="D519" s="2"/>
     </row>
-    <row r="520" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="520" spans="4:4" ht="13.2">
       <c r="D520" s="2"/>
     </row>
-    <row r="521" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="521" spans="4:4" ht="13.2">
       <c r="D521" s="2"/>
     </row>
-    <row r="522" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="522" spans="4:4" ht="13.2">
       <c r="D522" s="2"/>
     </row>
-    <row r="523" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="523" spans="4:4" ht="13.2">
       <c r="D523" s="2"/>
     </row>
-    <row r="524" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="524" spans="4:4" ht="13.2">
       <c r="D524" s="2"/>
     </row>
-    <row r="525" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="525" spans="4:4" ht="13.2">
       <c r="D525" s="2"/>
     </row>
-    <row r="526" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="526" spans="4:4" ht="13.2">
       <c r="D526" s="2"/>
     </row>
-    <row r="527" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="527" spans="4:4" ht="13.2">
       <c r="D527" s="2"/>
     </row>
-    <row r="528" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="528" spans="4:4" ht="13.2">
       <c r="D528" s="2"/>
     </row>
-    <row r="529" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="529" spans="4:4" ht="13.2">
       <c r="D529" s="2"/>
     </row>
-    <row r="530" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="530" spans="4:4" ht="13.2">
       <c r="D530" s="2"/>
     </row>
-    <row r="531" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="531" spans="4:4" ht="13.2">
       <c r="D531" s="2"/>
     </row>
-    <row r="532" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="532" spans="4:4" ht="13.2">
       <c r="D532" s="2"/>
     </row>
-    <row r="533" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="533" spans="4:4" ht="13.2">
       <c r="D533" s="2"/>
     </row>
-    <row r="534" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="534" spans="4:4" ht="13.2">
       <c r="D534" s="2"/>
     </row>
-    <row r="535" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="535" spans="4:4" ht="13.2">
       <c r="D535" s="2"/>
     </row>
-    <row r="536" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="536" spans="4:4" ht="13.2">
       <c r="D536" s="2"/>
     </row>
-    <row r="537" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="537" spans="4:4" ht="13.2">
       <c r="D537" s="2"/>
     </row>
-    <row r="538" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="538" spans="4:4" ht="13.2">
       <c r="D538" s="2"/>
     </row>
-    <row r="539" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="539" spans="4:4" ht="13.2">
       <c r="D539" s="2"/>
     </row>
-    <row r="540" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="540" spans="4:4" ht="13.2">
       <c r="D540" s="2"/>
     </row>
-    <row r="541" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="541" spans="4:4" ht="13.2">
       <c r="D541" s="2"/>
     </row>
-    <row r="542" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="542" spans="4:4" ht="13.2">
       <c r="D542" s="2"/>
     </row>
-    <row r="543" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="543" spans="4:4" ht="13.2">
       <c r="D543" s="2"/>
     </row>
-    <row r="544" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="544" spans="4:4" ht="13.2">
       <c r="D544" s="2"/>
     </row>
-    <row r="545" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="545" spans="4:4" ht="13.2">
       <c r="D545" s="2"/>
     </row>
-    <row r="546" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="546" spans="4:4" ht="13.2">
       <c r="D546" s="2"/>
     </row>
-    <row r="547" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="547" spans="4:4" ht="13.2">
       <c r="D547" s="2"/>
     </row>
-    <row r="548" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="548" spans="4:4" ht="13.2">
       <c r="D548" s="2"/>
     </row>
-    <row r="549" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="549" spans="4:4" ht="13.2">
       <c r="D549" s="2"/>
     </row>
-    <row r="550" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="550" spans="4:4" ht="13.2">
       <c r="D550" s="2"/>
     </row>
-    <row r="551" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="551" spans="4:4" ht="13.2">
       <c r="D551" s="2"/>
     </row>
-    <row r="552" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="552" spans="4:4" ht="13.2">
       <c r="D552" s="2"/>
     </row>
-    <row r="553" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="553" spans="4:4" ht="13.2">
       <c r="D553" s="2"/>
     </row>
-    <row r="554" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="554" spans="4:4" ht="13.2">
       <c r="D554" s="2"/>
     </row>
-    <row r="555" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="555" spans="4:4" ht="13.2">
       <c r="D555" s="2"/>
     </row>
-    <row r="556" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="556" spans="4:4" ht="13.2">
       <c r="D556" s="2"/>
     </row>
-    <row r="557" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="557" spans="4:4" ht="13.2">
       <c r="D557" s="2"/>
     </row>
-    <row r="558" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="558" spans="4:4" ht="13.2">
       <c r="D558" s="2"/>
     </row>
-    <row r="559" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="559" spans="4:4" ht="13.2">
       <c r="D559" s="2"/>
     </row>
-    <row r="560" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="560" spans="4:4" ht="13.2">
       <c r="D560" s="2"/>
     </row>
-    <row r="561" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="561" spans="4:4" ht="13.2">
       <c r="D561" s="2"/>
     </row>
-    <row r="562" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="562" spans="4:4" ht="13.2">
       <c r="D562" s="2"/>
     </row>
-    <row r="563" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="563" spans="4:4" ht="13.2">
       <c r="D563" s="2"/>
     </row>
-    <row r="564" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="564" spans="4:4" ht="13.2">
       <c r="D564" s="2"/>
     </row>
-    <row r="565" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="565" spans="4:4" ht="13.2">
       <c r="D565" s="2"/>
     </row>
-    <row r="566" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="566" spans="4:4" ht="13.2">
       <c r="D566" s="2"/>
     </row>
-    <row r="567" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="567" spans="4:4" ht="13.2">
       <c r="D567" s="2"/>
     </row>
-    <row r="568" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="568" spans="4:4" ht="13.2">
       <c r="D568" s="2"/>
     </row>
-    <row r="569" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="569" spans="4:4" ht="13.2">
       <c r="D569" s="2"/>
     </row>
-    <row r="570" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="570" spans="4:4" ht="13.2">
       <c r="D570" s="2"/>
     </row>
-    <row r="571" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="571" spans="4:4" ht="13.2">
       <c r="D571" s="2"/>
     </row>
-    <row r="572" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="572" spans="4:4" ht="13.2">
       <c r="D572" s="2"/>
     </row>
-    <row r="573" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="573" spans="4:4" ht="13.2">
       <c r="D573" s="2"/>
     </row>
-    <row r="574" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="574" spans="4:4" ht="13.2">
       <c r="D574" s="2"/>
     </row>
-    <row r="575" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="575" spans="4:4" ht="13.2">
       <c r="D575" s="2"/>
     </row>
-    <row r="576" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="576" spans="4:4" ht="13.2">
       <c r="D576" s="2"/>
     </row>
-    <row r="577" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="577" spans="4:4" ht="13.2">
       <c r="D577" s="2"/>
     </row>
-    <row r="578" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="578" spans="4:4" ht="13.2">
       <c r="D578" s="2"/>
     </row>
-    <row r="579" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="579" spans="4:4" ht="13.2">
       <c r="D579" s="2"/>
     </row>
-    <row r="580" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="580" spans="4:4" ht="13.2">
       <c r="D580" s="2"/>
     </row>
-    <row r="581" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="581" spans="4:4" ht="13.2">
       <c r="D581" s="2"/>
     </row>
-    <row r="582" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="582" spans="4:4" ht="13.2">
       <c r="D582" s="2"/>
     </row>
-    <row r="583" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="583" spans="4:4" ht="13.2">
       <c r="D583" s="2"/>
     </row>
-    <row r="584" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="584" spans="4:4" ht="13.2">
       <c r="D584" s="2"/>
     </row>
-    <row r="585" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="585" spans="4:4" ht="13.2">
       <c r="D585" s="2"/>
     </row>
-    <row r="586" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="586" spans="4:4" ht="13.2">
       <c r="D586" s="2"/>
     </row>
-    <row r="587" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="587" spans="4:4" ht="13.2">
       <c r="D587" s="2"/>
     </row>
-    <row r="588" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="588" spans="4:4" ht="13.2">
       <c r="D588" s="2"/>
     </row>
-    <row r="589" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="589" spans="4:4" ht="13.2">
       <c r="D589" s="2"/>
     </row>
-    <row r="590" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="590" spans="4:4" ht="13.2">
       <c r="D590" s="2"/>
     </row>
-    <row r="591" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="591" spans="4:4" ht="13.2">
       <c r="D591" s="2"/>
     </row>
-    <row r="592" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="592" spans="4:4" ht="13.2">
       <c r="D592" s="2"/>
     </row>
-    <row r="593" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="593" spans="4:4" ht="13.2">
       <c r="D593" s="2"/>
     </row>
-    <row r="594" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="594" spans="4:4" ht="13.2">
       <c r="D594" s="2"/>
     </row>
-    <row r="595" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="595" spans="4:4" ht="13.2">
       <c r="D595" s="2"/>
     </row>
-    <row r="596" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="596" spans="4:4" ht="13.2">
       <c r="D596" s="2"/>
     </row>
-    <row r="597" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="597" spans="4:4" ht="13.2">
       <c r="D597" s="2"/>
     </row>
-    <row r="598" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="598" spans="4:4" ht="13.2">
       <c r="D598" s="2"/>
     </row>
-    <row r="599" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="599" spans="4:4" ht="13.2">
       <c r="D599" s="2"/>
     </row>
-    <row r="600" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="600" spans="4:4" ht="13.2">
       <c r="D600" s="2"/>
     </row>
-    <row r="601" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="601" spans="4:4" ht="13.2">
       <c r="D601" s="2"/>
     </row>
-    <row r="602" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="602" spans="4:4" ht="13.2">
       <c r="D602" s="2"/>
     </row>
-    <row r="603" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="603" spans="4:4" ht="13.2">
       <c r="D603" s="2"/>
     </row>
-    <row r="604" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="604" spans="4:4" ht="13.2">
       <c r="D604" s="2"/>
     </row>
-    <row r="605" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="605" spans="4:4" ht="13.2">
       <c r="D605" s="2"/>
     </row>
-    <row r="606" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="606" spans="4:4" ht="13.2">
       <c r="D606" s="2"/>
     </row>
-    <row r="607" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="607" spans="4:4" ht="13.2">
       <c r="D607" s="2"/>
     </row>
-    <row r="608" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="608" spans="4:4" ht="13.2">
       <c r="D608" s="2"/>
     </row>
-    <row r="609" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="609" spans="4:4" ht="13.2">
       <c r="D609" s="2"/>
     </row>
-    <row r="610" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="610" spans="4:4" ht="13.2">
       <c r="D610" s="2"/>
     </row>
-    <row r="611" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="611" spans="4:4" ht="13.2">
       <c r="D611" s="2"/>
     </row>
-    <row r="612" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="612" spans="4:4" ht="13.2">
       <c r="D612" s="2"/>
     </row>
-    <row r="613" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="613" spans="4:4" ht="13.2">
       <c r="D613" s="2"/>
     </row>
-    <row r="614" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="614" spans="4:4" ht="13.2">
       <c r="D614" s="2"/>
     </row>
-    <row r="615" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="615" spans="4:4" ht="13.2">
       <c r="D615" s="2"/>
     </row>
-    <row r="616" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="616" spans="4:4" ht="13.2">
       <c r="D616" s="2"/>
     </row>
-    <row r="617" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="617" spans="4:4" ht="13.2">
       <c r="D617" s="2"/>
     </row>
-    <row r="618" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="618" spans="4:4" ht="13.2">
       <c r="D618" s="2"/>
     </row>
-    <row r="619" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="619" spans="4:4" ht="13.2">
       <c r="D619" s="2"/>
     </row>
-    <row r="620" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="620" spans="4:4" ht="13.2">
       <c r="D620" s="2"/>
     </row>
-    <row r="621" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="621" spans="4:4" ht="13.2">
       <c r="D621" s="2"/>
     </row>
-    <row r="622" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="622" spans="4:4" ht="13.2">
       <c r="D622" s="2"/>
     </row>
-    <row r="623" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="623" spans="4:4" ht="13.2">
       <c r="D623" s="2"/>
     </row>
-    <row r="624" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="624" spans="4:4" ht="13.2">
       <c r="D624" s="2"/>
     </row>
-    <row r="625" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="625" spans="4:4" ht="13.2">
       <c r="D625" s="2"/>
     </row>
-    <row r="626" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="626" spans="4:4" ht="13.2">
       <c r="D626" s="2"/>
     </row>
-    <row r="627" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="627" spans="4:4" ht="13.2">
       <c r="D627" s="2"/>
     </row>
-    <row r="628" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="628" spans="4:4" ht="13.2">
       <c r="D628" s="2"/>
     </row>
-    <row r="629" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="629" spans="4:4" ht="13.2">
       <c r="D629" s="2"/>
     </row>
-    <row r="630" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="630" spans="4:4" ht="13.2">
       <c r="D630" s="2"/>
     </row>
-    <row r="631" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="631" spans="4:4" ht="13.2">
       <c r="D631" s="2"/>
     </row>
-    <row r="632" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="632" spans="4:4" ht="13.2">
       <c r="D632" s="2"/>
     </row>
-    <row r="633" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="633" spans="4:4" ht="13.2">
       <c r="D633" s="2"/>
     </row>
-    <row r="634" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="634" spans="4:4" ht="13.2">
       <c r="D634" s="2"/>
     </row>
-    <row r="635" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="635" spans="4:4" ht="13.2">
       <c r="D635" s="2"/>
     </row>
-    <row r="636" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="636" spans="4:4" ht="13.2">
       <c r="D636" s="2"/>
     </row>
-    <row r="637" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="637" spans="4:4" ht="13.2">
       <c r="D637" s="2"/>
     </row>
-    <row r="638" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="638" spans="4:4" ht="13.2">
       <c r="D638" s="2"/>
     </row>
-    <row r="639" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="639" spans="4:4" ht="13.2">
       <c r="D639" s="2"/>
     </row>
-    <row r="640" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="640" spans="4:4" ht="13.2">
       <c r="D640" s="2"/>
     </row>
-    <row r="641" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="641" spans="4:4" ht="13.2">
       <c r="D641" s="2"/>
     </row>
-    <row r="642" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="642" spans="4:4" ht="13.2">
       <c r="D642" s="2"/>
     </row>
-    <row r="643" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="643" spans="4:4" ht="13.2">
       <c r="D643" s="2"/>
     </row>
-    <row r="644" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="644" spans="4:4" ht="13.2">
       <c r="D644" s="2"/>
     </row>
-    <row r="645" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="645" spans="4:4" ht="13.2">
       <c r="D645" s="2"/>
     </row>
-    <row r="646" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="646" spans="4:4" ht="13.2">
       <c r="D646" s="2"/>
     </row>
-    <row r="647" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="647" spans="4:4" ht="13.2">
       <c r="D647" s="2"/>
     </row>
-    <row r="648" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="648" spans="4:4" ht="13.2">
       <c r="D648" s="2"/>
     </row>
-    <row r="649" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="649" spans="4:4" ht="13.2">
       <c r="D649" s="2"/>
     </row>
-    <row r="650" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="650" spans="4:4" ht="13.2">
       <c r="D650" s="2"/>
     </row>
-    <row r="651" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="651" spans="4:4" ht="13.2">
       <c r="D651" s="2"/>
     </row>
-    <row r="652" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="652" spans="4:4" ht="13.2">
       <c r="D652" s="2"/>
     </row>
-    <row r="653" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="653" spans="4:4" ht="13.2">
       <c r="D653" s="2"/>
     </row>
-    <row r="654" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="654" spans="4:4" ht="13.2">
       <c r="D654" s="2"/>
     </row>
-    <row r="655" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="655" spans="4:4" ht="13.2">
       <c r="D655" s="2"/>
     </row>
-    <row r="656" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="656" spans="4:4" ht="13.2">
       <c r="D656" s="2"/>
     </row>
-    <row r="657" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="657" spans="4:4" ht="13.2">
       <c r="D657" s="2"/>
     </row>
-    <row r="658" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="658" spans="4:4" ht="13.2">
       <c r="D658" s="2"/>
     </row>
-    <row r="659" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="659" spans="4:4" ht="13.2">
       <c r="D659" s="2"/>
     </row>
-    <row r="660" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="660" spans="4:4" ht="13.2">
       <c r="D660" s="2"/>
     </row>
-    <row r="661" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="661" spans="4:4" ht="13.2">
       <c r="D661" s="2"/>
     </row>
-    <row r="662" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="662" spans="4:4" ht="13.2">
       <c r="D662" s="2"/>
     </row>
-    <row r="663" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="663" spans="4:4" ht="13.2">
       <c r="D663" s="2"/>
     </row>
-    <row r="664" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="664" spans="4:4" ht="13.2">
       <c r="D664" s="2"/>
     </row>
-    <row r="665" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="665" spans="4:4" ht="13.2">
       <c r="D665" s="2"/>
     </row>
-    <row r="666" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="666" spans="4:4" ht="13.2">
       <c r="D666" s="2"/>
     </row>
-    <row r="667" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="667" spans="4:4" ht="13.2">
       <c r="D667" s="2"/>
     </row>
-    <row r="668" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="668" spans="4:4" ht="13.2">
       <c r="D668" s="2"/>
     </row>
-    <row r="669" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="669" spans="4:4" ht="13.2">
       <c r="D669" s="2"/>
     </row>
-    <row r="670" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="670" spans="4:4" ht="13.2">
       <c r="D670" s="2"/>
     </row>
-    <row r="671" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="671" spans="4:4" ht="13.2">
       <c r="D671" s="2"/>
     </row>
-    <row r="672" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="672" spans="4:4" ht="13.2">
       <c r="D672" s="2"/>
     </row>
-    <row r="673" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="673" spans="4:4" ht="13.2">
       <c r="D673" s="2"/>
     </row>
-    <row r="674" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="674" spans="4:4" ht="13.2">
       <c r="D674" s="2"/>
     </row>
-    <row r="675" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="675" spans="4:4" ht="13.2">
       <c r="D675" s="2"/>
     </row>
-    <row r="676" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="676" spans="4:4" ht="13.2">
       <c r="D676" s="2"/>
     </row>
-    <row r="677" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="677" spans="4:4" ht="13.2">
       <c r="D677" s="2"/>
     </row>
-    <row r="678" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="678" spans="4:4" ht="13.2">
       <c r="D678" s="2"/>
     </row>
-    <row r="679" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="679" spans="4:4" ht="13.2">
       <c r="D679" s="2"/>
     </row>
-    <row r="680" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="680" spans="4:4" ht="13.2">
       <c r="D680" s="2"/>
     </row>
-    <row r="681" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="681" spans="4:4" ht="13.2">
       <c r="D681" s="2"/>
     </row>
-    <row r="682" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="682" spans="4:4" ht="13.2">
       <c r="D682" s="2"/>
     </row>
-    <row r="683" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="683" spans="4:4" ht="13.2">
       <c r="D683" s="2"/>
     </row>
-    <row r="684" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="684" spans="4:4" ht="13.2">
       <c r="D684" s="2"/>
     </row>
-    <row r="685" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="685" spans="4:4" ht="13.2">
       <c r="D685" s="2"/>
     </row>
-    <row r="686" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="686" spans="4:4" ht="13.2">
       <c r="D686" s="2"/>
     </row>
-    <row r="687" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="687" spans="4:4" ht="13.2">
       <c r="D687" s="2"/>
     </row>
-    <row r="688" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="688" spans="4:4" ht="13.2">
       <c r="D688" s="2"/>
     </row>
-    <row r="689" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="689" spans="4:4" ht="13.2">
       <c r="D689" s="2"/>
     </row>
-    <row r="690" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="690" spans="4:4" ht="13.2">
       <c r="D690" s="2"/>
     </row>
-    <row r="691" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="691" spans="4:4" ht="13.2">
       <c r="D691" s="2"/>
     </row>
-    <row r="692" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="692" spans="4:4" ht="13.2">
       <c r="D692" s="2"/>
     </row>
-    <row r="693" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="693" spans="4:4" ht="13.2">
       <c r="D693" s="2"/>
     </row>
-    <row r="694" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="694" spans="4:4" ht="13.2">
       <c r="D694" s="2"/>
     </row>
-    <row r="695" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="695" spans="4:4" ht="13.2">
       <c r="D695" s="2"/>
     </row>
-    <row r="696" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="696" spans="4:4" ht="13.2">
       <c r="D696" s="2"/>
     </row>
-    <row r="697" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="697" spans="4:4" ht="13.2">
       <c r="D697" s="2"/>
     </row>
-    <row r="698" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="698" spans="4:4" ht="13.2">
       <c r="D698" s="2"/>
     </row>
-    <row r="699" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="699" spans="4:4" ht="13.2">
       <c r="D699" s="2"/>
     </row>
-    <row r="700" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="700" spans="4:4" ht="13.2">
       <c r="D700" s="2"/>
     </row>
-    <row r="701" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="701" spans="4:4" ht="13.2">
       <c r="D701" s="2"/>
     </row>
-    <row r="702" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="702" spans="4:4" ht="13.2">
       <c r="D702" s="2"/>
     </row>
-    <row r="703" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="703" spans="4:4" ht="13.2">
       <c r="D703" s="2"/>
     </row>
-    <row r="704" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="704" spans="4:4" ht="13.2">
       <c r="D704" s="2"/>
     </row>
-    <row r="705" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="705" spans="4:4" ht="13.2">
       <c r="D705" s="2"/>
     </row>
-    <row r="706" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="706" spans="4:4" ht="13.2">
       <c r="D706" s="2"/>
     </row>
-    <row r="707" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="707" spans="4:4" ht="13.2">
       <c r="D707" s="2"/>
     </row>
-    <row r="708" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="708" spans="4:4" ht="13.2">
       <c r="D708" s="2"/>
     </row>
-    <row r="709" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="709" spans="4:4" ht="13.2">
       <c r="D709" s="2"/>
     </row>
-    <row r="710" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="710" spans="4:4" ht="13.2">
       <c r="D710" s="2"/>
     </row>
-    <row r="711" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="711" spans="4:4" ht="13.2">
       <c r="D711" s="2"/>
     </row>
-    <row r="712" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="712" spans="4:4" ht="13.2">
       <c r="D712" s="2"/>
     </row>
-    <row r="713" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="713" spans="4:4" ht="13.2">
       <c r="D713" s="2"/>
     </row>
-    <row r="714" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="714" spans="4:4" ht="13.2">
       <c r="D714" s="2"/>
     </row>
-    <row r="715" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="715" spans="4:4" ht="13.2">
       <c r="D715" s="2"/>
     </row>
-    <row r="716" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="716" spans="4:4" ht="13.2">
       <c r="D716" s="2"/>
     </row>
-    <row r="717" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="717" spans="4:4" ht="13.2">
       <c r="D717" s="2"/>
     </row>
-    <row r="718" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="718" spans="4:4" ht="13.2">
       <c r="D718" s="2"/>
     </row>
-    <row r="719" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="719" spans="4:4" ht="13.2">
       <c r="D719" s="2"/>
     </row>
-    <row r="720" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="720" spans="4:4" ht="13.2">
       <c r="D720" s="2"/>
     </row>
-    <row r="721" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="721" spans="4:4" ht="13.2">
       <c r="D721" s="2"/>
     </row>
-    <row r="722" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="722" spans="4:4" ht="13.2">
       <c r="D722" s="2"/>
     </row>
-    <row r="723" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="723" spans="4:4" ht="13.2">
       <c r="D723" s="2"/>
     </row>
-    <row r="724" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="724" spans="4:4" ht="13.2">
       <c r="D724" s="2"/>
     </row>
-    <row r="725" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="725" spans="4:4" ht="13.2">
       <c r="D725" s="2"/>
     </row>
-    <row r="726" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="726" spans="4:4" ht="13.2">
       <c r="D726" s="2"/>
     </row>
-    <row r="727" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="727" spans="4:4" ht="13.2">
       <c r="D727" s="2"/>
     </row>
-    <row r="728" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="728" spans="4:4" ht="13.2">
       <c r="D728" s="2"/>
     </row>
-    <row r="729" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="729" spans="4:4" ht="13.2">
       <c r="D729" s="2"/>
     </row>
-    <row r="730" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="730" spans="4:4" ht="13.2">
       <c r="D730" s="2"/>
     </row>
-    <row r="731" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="731" spans="4:4" ht="13.2">
       <c r="D731" s="2"/>
     </row>
-    <row r="732" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="732" spans="4:4" ht="13.2">
       <c r="D732" s="2"/>
     </row>
-    <row r="733" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="733" spans="4:4" ht="13.2">
       <c r="D733" s="2"/>
     </row>
-    <row r="734" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="734" spans="4:4" ht="13.2">
       <c r="D734" s="2"/>
     </row>
-    <row r="735" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="735" spans="4:4" ht="13.2">
       <c r="D735" s="2"/>
     </row>
-    <row r="736" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="736" spans="4:4" ht="13.2">
       <c r="D736" s="2"/>
     </row>
-    <row r="737" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="737" spans="4:4" ht="13.2">
       <c r="D737" s="2"/>
     </row>
-    <row r="738" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="738" spans="4:4" ht="13.2">
       <c r="D738" s="2"/>
     </row>
-    <row r="739" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="739" spans="4:4" ht="13.2">
       <c r="D739" s="2"/>
     </row>
-    <row r="740" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="740" spans="4:4" ht="13.2">
       <c r="D740" s="2"/>
     </row>
-    <row r="741" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="741" spans="4:4" ht="13.2">
       <c r="D741" s="2"/>
     </row>
-    <row r="742" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="742" spans="4:4" ht="13.2">
       <c r="D742" s="2"/>
     </row>
-    <row r="743" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="743" spans="4:4" ht="13.2">
       <c r="D743" s="2"/>
     </row>
-    <row r="744" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="744" spans="4:4" ht="13.2">
       <c r="D744" s="2"/>
     </row>
-    <row r="745" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="745" spans="4:4" ht="13.2">
       <c r="D745" s="2"/>
     </row>
-    <row r="746" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="746" spans="4:4" ht="13.2">
       <c r="D746" s="2"/>
     </row>
-    <row r="747" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="747" spans="4:4" ht="13.2">
       <c r="D747" s="2"/>
     </row>
-    <row r="748" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="748" spans="4:4" ht="13.2">
       <c r="D748" s="2"/>
     </row>
-    <row r="749" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="749" spans="4:4" ht="13.2">
       <c r="D749" s="2"/>
     </row>
-    <row r="750" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="750" spans="4:4" ht="13.2">
       <c r="D750" s="2"/>
     </row>
-    <row r="751" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="751" spans="4:4" ht="13.2">
       <c r="D751" s="2"/>
     </row>
   </sheetData>
@@ -5962,44 +5962,44 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="containsText" dxfId="11" priority="22" operator="containsText" text="female">
+    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="female">
       <formula>NOT(ISERROR(SEARCH(("female"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="23" operator="containsText" text="male">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="male">
       <formula>NOT(ISERROR(SEARCH(("male"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D117">
-    <cfRule type="containsText" dxfId="9" priority="20" operator="containsText" text="both">
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="both">
       <formula>NOT(ISERROR(SEARCH(("both"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:D117">
-    <cfRule type="containsText" dxfId="8" priority="19" operator="containsText" text="female">
+    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="female">
       <formula>NOT(ISERROR(SEARCH(("female"),(D14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:D145">
-    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="male">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="male">
       <formula>NOT(ISERROR(SEARCH(("male"),(D14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D118:D145">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="both">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="both">
       <formula>NOT(ISERROR(SEARCH(("both"),(D118))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="female">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="female">
       <formula>NOT(ISERROR(SEARCH(("female"),(D118))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="containsText" dxfId="4" priority="25" operator="containsText" text="both">
+    <cfRule type="containsText" dxfId="12" priority="25" operator="containsText" text="both">
       <formula>NOT(ISERROR(SEARCH(("both"),(E1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="26" operator="containsText" text="female">
+    <cfRule type="containsText" dxfId="11" priority="26" operator="containsText" text="female">
       <formula>NOT(ISERROR(SEARCH(("female"),(E1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="27" operator="containsText" text="male">
+    <cfRule type="containsText" dxfId="10" priority="27" operator="containsText" text="male">
       <formula>NOT(ISERROR(SEARCH(("male"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>